<commit_message>
more changes on master branch
</commit_message>
<xml_diff>
--- a/src/test/resources/datatable/login.xlsx
+++ b/src/test/resources/datatable/login.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>password</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>yuvi@666</t>
+  </si>
+  <si>
+    <t>TC_LoginTest_02</t>
+  </si>
+  <si>
+    <t>asdfasdf</t>
   </si>
 </sst>
 </file>
@@ -427,10 +433,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,10 +474,26 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3" display="yuvi@666"/>
+    <hyperlink ref="C3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>